<commit_message>
Added coaches handout file
</commit_message>
<xml_diff>
--- a/PlansYear2.xlsx
+++ b/PlansYear2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxwell Dulin\Desktop\CTF\GonzagaCTF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxwell Dulin\Desktop\CTF\SMC2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A640D286-CBEE-4F4F-9CD4-6F19ECB14B5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC777DD3-1603-41AD-AD26-44CF30944485}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="820" activeTab="6" xr2:uid="{FCFD1292-8C82-47E9-ABE8-C58E7364A0F6}"/>
+    <workbookView xWindow="17724" yWindow="5004" windowWidth="7500" windowHeight="6000" tabRatio="820" activeTab="2" xr2:uid="{FCFD1292-8C82-47E9-ABE8-C58E7364A0F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Challenge Flags" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="147">
   <si>
     <t>Challenge Name</t>
   </si>
@@ -478,6 +478,9 @@
   </si>
   <si>
     <t>Log Analysis</t>
+  </si>
+  <si>
+    <t>Waiting on Corey's…</t>
   </si>
 </sst>
 </file>
@@ -896,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88EF27B0-3FC8-4B4F-B891-E12E90045284}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:C40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1398,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3FDB87-32B4-4558-B40D-F27094BD6748}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1538,7 +1541,7 @@
       <c r="A9" t="s">
         <v>92</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C9">
@@ -1612,21 +1615,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384ACA9D-86DA-4D4C-A0D1-2EB8EF2C2B4E}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.21875" customWidth="1"/>
     <col min="2" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="5" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="105" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="105" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1640,16 +1643,13 @@
         <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>141</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1662,11 +1662,11 @@
       <c r="D2">
         <v>6</v>
       </c>
-      <c r="F2">
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1679,11 +1679,11 @@
       <c r="D4">
         <v>4</v>
       </c>
-      <c r="F4">
+      <c r="E4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1696,14 +1696,14 @@
       <c r="D5">
         <v>10</v>
       </c>
-      <c r="F5">
+      <c r="E5">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1716,11 +1716,11 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="E6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1733,11 +1733,11 @@
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="F7">
+      <c r="E7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1750,14 +1750,14 @@
       <c r="D8">
         <v>5</v>
       </c>
-      <c r="F8">
+      <c r="E8">
         <v>2</v>
       </c>
-      <c r="G8" t="s">
+      <c r="F8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1770,11 +1770,11 @@
       <c r="D9">
         <v>3</v>
       </c>
-      <c r="F9">
+      <c r="E9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1787,11 +1787,11 @@
       <c r="D10">
         <v>7</v>
       </c>
-      <c r="F10">
+      <c r="E10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1804,14 +1804,14 @@
       <c r="D11">
         <v>7</v>
       </c>
-      <c r="F11">
+      <c r="E11">
         <v>2</v>
       </c>
-      <c r="G11" t="s">
+      <c r="F11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>134</v>
       </c>
@@ -1824,22 +1824,22 @@
       <c r="D13">
         <v>10</v>
       </c>
-      <c r="F13">
+      <c r="E13">
         <v>2</v>
       </c>
-      <c r="G13" t="s">
+      <c r="F13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>94</v>
       </c>
       <c r="B18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>95</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>90</v>
       </c>
@@ -1855,15 +1855,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>96</v>
       </c>
       <c r="B21">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -1871,29 +1871,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>97</v>
       </c>
       <c r="B23">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>145</v>
       </c>
       <c r="B24">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B25" s="1">
         <f>SUM(B18:B24)</f>
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2325,7 +2328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194E8DA5-013C-4ECA-8E95-1E5C3A0D9071}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>